<commit_message>
Fixed confirming tesla exists in fidelity issue
</commit_message>
<xml_diff>
--- a/Tesla Stock Logs.xlsx
+++ b/Tesla Stock Logs.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11475" windowWidth="21570" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy\-mm\-dd" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,13 +48,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -351,17 +350,13 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="16"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="18"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="17.85546875"/>
-    <col bestFit="1" customWidth="1" max="6" min="5" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -425,7 +420,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>43618</v>
       </c>
       <c r="B3" t="n">

</xml_diff>